<commit_message>
Me despido de SHE, se lo cedo al señor William
</commit_message>
<xml_diff>
--- a/public/formatos/GTH_F_060__FORMATO_LEGALIZACION_DE_HORAS_EXTRAS_RECARGOS_NOCTURNOS_DOMIN....xlsx
+++ b/public/formatos/GTH_F_060__FORMATO_LEGALIZACION_DE_HORAS_EXTRAS_RECARGOS_NOCTURNOS_DOMIN....xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\she\formatos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\she\public\formatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1428,8 +1428,143 @@
     <xf numFmtId="0" fontId="15" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1449,27 +1584,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1494,172 +1608,43 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1668,38 +1653,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2119,8 +2119,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Z45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38:Z38"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Z36" sqref="B13:Z36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3224,363 +3224,363 @@
   <sheetData>
     <row r="1" spans="2:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:26" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="65"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="66"/>
-      <c r="K2" s="66"/>
-      <c r="L2" s="66"/>
-      <c r="M2" s="66"/>
-      <c r="N2" s="66"/>
-      <c r="O2" s="66"/>
-      <c r="P2" s="66"/>
-      <c r="Q2" s="66"/>
-      <c r="R2" s="66"/>
-      <c r="S2" s="66"/>
-      <c r="T2" s="66"/>
-      <c r="U2" s="66"/>
-      <c r="V2" s="66"/>
-      <c r="W2" s="66"/>
-      <c r="X2" s="66"/>
-      <c r="Y2" s="66"/>
-      <c r="Z2" s="67"/>
+      <c r="B2" s="110"/>
+      <c r="C2" s="111"/>
+      <c r="D2" s="111"/>
+      <c r="E2" s="111"/>
+      <c r="F2" s="111"/>
+      <c r="G2" s="111"/>
+      <c r="H2" s="111"/>
+      <c r="I2" s="111"/>
+      <c r="J2" s="111"/>
+      <c r="K2" s="111"/>
+      <c r="L2" s="111"/>
+      <c r="M2" s="111"/>
+      <c r="N2" s="111"/>
+      <c r="O2" s="111"/>
+      <c r="P2" s="111"/>
+      <c r="Q2" s="111"/>
+      <c r="R2" s="111"/>
+      <c r="S2" s="111"/>
+      <c r="T2" s="111"/>
+      <c r="U2" s="111"/>
+      <c r="V2" s="111"/>
+      <c r="W2" s="111"/>
+      <c r="X2" s="111"/>
+      <c r="Y2" s="111"/>
+      <c r="Z2" s="112"/>
     </row>
     <row r="3" spans="2:26" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="68"/>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="69"/>
-      <c r="H3" s="69"/>
-      <c r="I3" s="69"/>
-      <c r="J3" s="69"/>
-      <c r="K3" s="69"/>
-      <c r="L3" s="69"/>
-      <c r="M3" s="69"/>
-      <c r="N3" s="69"/>
-      <c r="O3" s="69"/>
-      <c r="P3" s="69"/>
-      <c r="Q3" s="69"/>
-      <c r="R3" s="69"/>
-      <c r="S3" s="69"/>
-      <c r="T3" s="69"/>
-      <c r="U3" s="69"/>
-      <c r="V3" s="69"/>
-      <c r="W3" s="69"/>
-      <c r="X3" s="69"/>
-      <c r="Y3" s="69"/>
-      <c r="Z3" s="70"/>
+      <c r="B3" s="113"/>
+      <c r="C3" s="114"/>
+      <c r="D3" s="114"/>
+      <c r="E3" s="114"/>
+      <c r="F3" s="114"/>
+      <c r="G3" s="114"/>
+      <c r="H3" s="114"/>
+      <c r="I3" s="114"/>
+      <c r="J3" s="114"/>
+      <c r="K3" s="114"/>
+      <c r="L3" s="114"/>
+      <c r="M3" s="114"/>
+      <c r="N3" s="114"/>
+      <c r="O3" s="114"/>
+      <c r="P3" s="114"/>
+      <c r="Q3" s="114"/>
+      <c r="R3" s="114"/>
+      <c r="S3" s="114"/>
+      <c r="T3" s="114"/>
+      <c r="U3" s="114"/>
+      <c r="V3" s="114"/>
+      <c r="W3" s="114"/>
+      <c r="X3" s="114"/>
+      <c r="Y3" s="114"/>
+      <c r="Z3" s="115"/>
     </row>
     <row r="4" spans="2:26" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="82" t="s">
+      <c r="B4" s="120" t="s">
         <v>66</v>
       </c>
-      <c r="C4" s="83"/>
-      <c r="D4" s="83"/>
-      <c r="E4" s="83"/>
-      <c r="F4" s="83"/>
-      <c r="G4" s="83"/>
-      <c r="H4" s="83"/>
-      <c r="I4" s="83"/>
-      <c r="J4" s="83"/>
-      <c r="K4" s="83"/>
-      <c r="L4" s="83"/>
-      <c r="M4" s="83"/>
-      <c r="N4" s="83"/>
-      <c r="O4" s="83"/>
-      <c r="P4" s="83"/>
-      <c r="Q4" s="83"/>
-      <c r="R4" s="83"/>
-      <c r="S4" s="83"/>
-      <c r="T4" s="83"/>
-      <c r="U4" s="83"/>
-      <c r="V4" s="83"/>
-      <c r="W4" s="83"/>
-      <c r="X4" s="78" t="s">
+      <c r="C4" s="121"/>
+      <c r="D4" s="121"/>
+      <c r="E4" s="121"/>
+      <c r="F4" s="121"/>
+      <c r="G4" s="121"/>
+      <c r="H4" s="121"/>
+      <c r="I4" s="121"/>
+      <c r="J4" s="121"/>
+      <c r="K4" s="121"/>
+      <c r="L4" s="121"/>
+      <c r="M4" s="121"/>
+      <c r="N4" s="121"/>
+      <c r="O4" s="121"/>
+      <c r="P4" s="121"/>
+      <c r="Q4" s="121"/>
+      <c r="R4" s="121"/>
+      <c r="S4" s="121"/>
+      <c r="T4" s="121"/>
+      <c r="U4" s="121"/>
+      <c r="V4" s="121"/>
+      <c r="W4" s="121"/>
+      <c r="X4" s="116" t="s">
         <v>64</v>
       </c>
-      <c r="Y4" s="78"/>
-      <c r="Z4" s="79"/>
+      <c r="Y4" s="116"/>
+      <c r="Z4" s="117"/>
     </row>
     <row r="5" spans="2:26" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="84"/>
-      <c r="C5" s="85"/>
-      <c r="D5" s="85"/>
-      <c r="E5" s="85"/>
-      <c r="F5" s="85"/>
-      <c r="G5" s="85"/>
-      <c r="H5" s="85"/>
-      <c r="I5" s="85"/>
-      <c r="J5" s="85"/>
-      <c r="K5" s="85"/>
-      <c r="L5" s="85"/>
-      <c r="M5" s="85"/>
-      <c r="N5" s="85"/>
-      <c r="O5" s="85"/>
-      <c r="P5" s="85"/>
-      <c r="Q5" s="85"/>
-      <c r="R5" s="85"/>
-      <c r="S5" s="85"/>
-      <c r="T5" s="85"/>
-      <c r="U5" s="85"/>
-      <c r="V5" s="85"/>
-      <c r="W5" s="85"/>
-      <c r="X5" s="80" t="s">
+      <c r="B5" s="122"/>
+      <c r="C5" s="123"/>
+      <c r="D5" s="123"/>
+      <c r="E5" s="123"/>
+      <c r="F5" s="123"/>
+      <c r="G5" s="123"/>
+      <c r="H5" s="123"/>
+      <c r="I5" s="123"/>
+      <c r="J5" s="123"/>
+      <c r="K5" s="123"/>
+      <c r="L5" s="123"/>
+      <c r="M5" s="123"/>
+      <c r="N5" s="123"/>
+      <c r="O5" s="123"/>
+      <c r="P5" s="123"/>
+      <c r="Q5" s="123"/>
+      <c r="R5" s="123"/>
+      <c r="S5" s="123"/>
+      <c r="T5" s="123"/>
+      <c r="U5" s="123"/>
+      <c r="V5" s="123"/>
+      <c r="W5" s="123"/>
+      <c r="X5" s="118" t="s">
         <v>63</v>
       </c>
-      <c r="Y5" s="80"/>
-      <c r="Z5" s="81"/>
+      <c r="Y5" s="118"/>
+      <c r="Z5" s="119"/>
     </row>
     <row r="6" spans="2:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="74" t="s">
+      <c r="B6" s="146" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="75"/>
-      <c r="D6" s="75"/>
-      <c r="E6" s="75"/>
-      <c r="F6" s="75"/>
-      <c r="G6" s="75"/>
-      <c r="H6" s="75"/>
-      <c r="I6" s="77"/>
-      <c r="J6" s="74" t="s">
+      <c r="C6" s="147"/>
+      <c r="D6" s="147"/>
+      <c r="E6" s="147"/>
+      <c r="F6" s="147"/>
+      <c r="G6" s="147"/>
+      <c r="H6" s="147"/>
+      <c r="I6" s="148"/>
+      <c r="J6" s="146" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="75"/>
-      <c r="L6" s="75"/>
-      <c r="M6" s="75"/>
-      <c r="N6" s="75"/>
-      <c r="O6" s="75"/>
-      <c r="P6" s="76"/>
-      <c r="Q6" s="71" t="s">
+      <c r="K6" s="147"/>
+      <c r="L6" s="147"/>
+      <c r="M6" s="147"/>
+      <c r="N6" s="147"/>
+      <c r="O6" s="147"/>
+      <c r="P6" s="149"/>
+      <c r="Q6" s="150" t="s">
         <v>9</v>
       </c>
-      <c r="R6" s="72"/>
-      <c r="S6" s="72"/>
-      <c r="T6" s="72"/>
-      <c r="U6" s="72"/>
-      <c r="V6" s="72"/>
-      <c r="W6" s="72"/>
-      <c r="X6" s="72"/>
-      <c r="Y6" s="72"/>
-      <c r="Z6" s="73"/>
+      <c r="R6" s="151"/>
+      <c r="S6" s="151"/>
+      <c r="T6" s="151"/>
+      <c r="U6" s="151"/>
+      <c r="V6" s="151"/>
+      <c r="W6" s="151"/>
+      <c r="X6" s="151"/>
+      <c r="Y6" s="151"/>
+      <c r="Z6" s="152"/>
     </row>
     <row r="7" spans="2:26" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="86"/>
-      <c r="C7" s="87"/>
-      <c r="D7" s="87"/>
-      <c r="E7" s="87"/>
-      <c r="F7" s="87"/>
-      <c r="G7" s="87"/>
-      <c r="H7" s="87"/>
-      <c r="I7" s="88"/>
-      <c r="J7" s="86"/>
-      <c r="K7" s="87"/>
-      <c r="L7" s="87"/>
-      <c r="M7" s="87"/>
-      <c r="N7" s="87"/>
-      <c r="O7" s="87"/>
-      <c r="P7" s="89"/>
-      <c r="Q7" s="90"/>
-      <c r="R7" s="91"/>
-      <c r="S7" s="91"/>
-      <c r="T7" s="91"/>
-      <c r="U7" s="91"/>
-      <c r="V7" s="91"/>
-      <c r="W7" s="91"/>
-      <c r="X7" s="91"/>
-      <c r="Y7" s="91"/>
-      <c r="Z7" s="92"/>
+      <c r="B7" s="139"/>
+      <c r="C7" s="140"/>
+      <c r="D7" s="140"/>
+      <c r="E7" s="140"/>
+      <c r="F7" s="140"/>
+      <c r="G7" s="140"/>
+      <c r="H7" s="140"/>
+      <c r="I7" s="141"/>
+      <c r="J7" s="139"/>
+      <c r="K7" s="140"/>
+      <c r="L7" s="140"/>
+      <c r="M7" s="140"/>
+      <c r="N7" s="140"/>
+      <c r="O7" s="140"/>
+      <c r="P7" s="142"/>
+      <c r="Q7" s="143"/>
+      <c r="R7" s="144"/>
+      <c r="S7" s="144"/>
+      <c r="T7" s="144"/>
+      <c r="U7" s="144"/>
+      <c r="V7" s="144"/>
+      <c r="W7" s="144"/>
+      <c r="X7" s="144"/>
+      <c r="Y7" s="144"/>
+      <c r="Z7" s="145"/>
     </row>
     <row r="8" spans="2:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="93" t="s">
+      <c r="B8" s="153" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="93"/>
-      <c r="D8" s="93"/>
-      <c r="E8" s="93"/>
-      <c r="F8" s="93"/>
-      <c r="G8" s="93" t="s">
+      <c r="C8" s="153"/>
+      <c r="D8" s="153"/>
+      <c r="E8" s="153"/>
+      <c r="F8" s="153"/>
+      <c r="G8" s="153" t="s">
         <v>40</v>
       </c>
-      <c r="H8" s="93"/>
-      <c r="I8" s="93"/>
-      <c r="J8" s="93"/>
-      <c r="K8" s="93"/>
-      <c r="L8" s="93"/>
-      <c r="M8" s="93"/>
-      <c r="N8" s="93"/>
-      <c r="O8" s="93" t="s">
+      <c r="H8" s="153"/>
+      <c r="I8" s="153"/>
+      <c r="J8" s="153"/>
+      <c r="K8" s="153"/>
+      <c r="L8" s="153"/>
+      <c r="M8" s="153"/>
+      <c r="N8" s="153"/>
+      <c r="O8" s="153" t="s">
         <v>24</v>
       </c>
-      <c r="P8" s="93"/>
-      <c r="Q8" s="93"/>
-      <c r="R8" s="93"/>
-      <c r="S8" s="93"/>
-      <c r="T8" s="93" t="s">
+      <c r="P8" s="153"/>
+      <c r="Q8" s="153"/>
+      <c r="R8" s="153"/>
+      <c r="S8" s="153"/>
+      <c r="T8" s="153" t="s">
         <v>39</v>
       </c>
-      <c r="U8" s="93"/>
-      <c r="V8" s="93"/>
-      <c r="W8" s="93"/>
-      <c r="X8" s="93"/>
-      <c r="Y8" s="93"/>
-      <c r="Z8" s="93"/>
+      <c r="U8" s="153"/>
+      <c r="V8" s="153"/>
+      <c r="W8" s="153"/>
+      <c r="X8" s="153"/>
+      <c r="Y8" s="153"/>
+      <c r="Z8" s="153"/>
     </row>
     <row r="9" spans="2:26" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="64"/>
-      <c r="C9" s="64"/>
-      <c r="D9" s="64"/>
-      <c r="E9" s="64"/>
-      <c r="F9" s="64"/>
-      <c r="G9" s="64"/>
-      <c r="H9" s="64"/>
-      <c r="I9" s="64"/>
-      <c r="J9" s="64"/>
-      <c r="K9" s="64"/>
-      <c r="L9" s="64"/>
-      <c r="M9" s="64"/>
-      <c r="N9" s="64"/>
-      <c r="O9" s="64"/>
-      <c r="P9" s="64"/>
-      <c r="Q9" s="64"/>
-      <c r="R9" s="64"/>
-      <c r="S9" s="64"/>
-      <c r="T9" s="64"/>
-      <c r="U9" s="64"/>
-      <c r="V9" s="64"/>
-      <c r="W9" s="64"/>
-      <c r="X9" s="64"/>
-      <c r="Y9" s="64"/>
-      <c r="Z9" s="64"/>
+      <c r="B9" s="154"/>
+      <c r="C9" s="154"/>
+      <c r="D9" s="154"/>
+      <c r="E9" s="154"/>
+      <c r="F9" s="154"/>
+      <c r="G9" s="154"/>
+      <c r="H9" s="154"/>
+      <c r="I9" s="154"/>
+      <c r="J9" s="154"/>
+      <c r="K9" s="154"/>
+      <c r="L9" s="154"/>
+      <c r="M9" s="154"/>
+      <c r="N9" s="154"/>
+      <c r="O9" s="154"/>
+      <c r="P9" s="154"/>
+      <c r="Q9" s="154"/>
+      <c r="R9" s="154"/>
+      <c r="S9" s="154"/>
+      <c r="T9" s="154"/>
+      <c r="U9" s="154"/>
+      <c r="V9" s="154"/>
+      <c r="W9" s="154"/>
+      <c r="X9" s="154"/>
+      <c r="Y9" s="154"/>
+      <c r="Z9" s="154"/>
     </row>
     <row r="10" spans="2:26" x14ac:dyDescent="0.2">
-      <c r="B10" s="137" t="s">
+      <c r="B10" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="131">
+      <c r="C10" s="70">
         <v>1201</v>
       </c>
-      <c r="D10" s="132"/>
-      <c r="E10" s="132"/>
-      <c r="F10" s="132"/>
-      <c r="G10" s="132"/>
-      <c r="H10" s="133"/>
-      <c r="I10" s="132">
+      <c r="D10" s="71"/>
+      <c r="E10" s="71"/>
+      <c r="F10" s="71"/>
+      <c r="G10" s="71"/>
+      <c r="H10" s="72"/>
+      <c r="I10" s="71">
         <v>1202</v>
       </c>
-      <c r="J10" s="132"/>
-      <c r="K10" s="132"/>
-      <c r="L10" s="132"/>
-      <c r="M10" s="132"/>
-      <c r="N10" s="132"/>
-      <c r="O10" s="131">
+      <c r="J10" s="71"/>
+      <c r="K10" s="71"/>
+      <c r="L10" s="71"/>
+      <c r="M10" s="71"/>
+      <c r="N10" s="71"/>
+      <c r="O10" s="70">
         <v>1204</v>
       </c>
-      <c r="P10" s="132"/>
-      <c r="Q10" s="132"/>
-      <c r="R10" s="132"/>
-      <c r="S10" s="132"/>
-      <c r="T10" s="133"/>
-      <c r="U10" s="132">
+      <c r="P10" s="71"/>
+      <c r="Q10" s="71"/>
+      <c r="R10" s="71"/>
+      <c r="S10" s="71"/>
+      <c r="T10" s="72"/>
+      <c r="U10" s="71">
         <v>1203</v>
       </c>
-      <c r="V10" s="132"/>
-      <c r="W10" s="132"/>
-      <c r="X10" s="132"/>
-      <c r="Y10" s="132"/>
-      <c r="Z10" s="133"/>
+      <c r="V10" s="71"/>
+      <c r="W10" s="71"/>
+      <c r="X10" s="71"/>
+      <c r="Y10" s="71"/>
+      <c r="Z10" s="72"/>
     </row>
     <row r="11" spans="2:26" x14ac:dyDescent="0.2">
-      <c r="B11" s="138"/>
-      <c r="C11" s="134" t="s">
+      <c r="B11" s="68"/>
+      <c r="C11" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="135"/>
-      <c r="E11" s="135"/>
-      <c r="F11" s="135"/>
-      <c r="G11" s="135"/>
-      <c r="H11" s="136"/>
-      <c r="I11" s="135" t="s">
+      <c r="D11" s="65"/>
+      <c r="E11" s="65"/>
+      <c r="F11" s="65"/>
+      <c r="G11" s="65"/>
+      <c r="H11" s="66"/>
+      <c r="I11" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="J11" s="135"/>
-      <c r="K11" s="135"/>
-      <c r="L11" s="135"/>
-      <c r="M11" s="135"/>
-      <c r="N11" s="135"/>
-      <c r="O11" s="134" t="s">
+      <c r="J11" s="65"/>
+      <c r="K11" s="65"/>
+      <c r="L11" s="65"/>
+      <c r="M11" s="65"/>
+      <c r="N11" s="65"/>
+      <c r="O11" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="P11" s="135"/>
-      <c r="Q11" s="135"/>
-      <c r="R11" s="135"/>
-      <c r="S11" s="135"/>
-      <c r="T11" s="136"/>
-      <c r="U11" s="135" t="s">
+      <c r="P11" s="65"/>
+      <c r="Q11" s="65"/>
+      <c r="R11" s="65"/>
+      <c r="S11" s="65"/>
+      <c r="T11" s="66"/>
+      <c r="U11" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="V11" s="135"/>
-      <c r="W11" s="135"/>
-      <c r="X11" s="135"/>
-      <c r="Y11" s="135"/>
-      <c r="Z11" s="136"/>
+      <c r="V11" s="65"/>
+      <c r="W11" s="65"/>
+      <c r="X11" s="65"/>
+      <c r="Y11" s="65"/>
+      <c r="Z11" s="66"/>
     </row>
     <row r="12" spans="2:26" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="139"/>
+      <c r="B12" s="69"/>
       <c r="C12" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="109" t="s">
+      <c r="E12" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="110"/>
-      <c r="G12" s="110"/>
-      <c r="H12" s="111"/>
+      <c r="F12" s="74"/>
+      <c r="G12" s="74"/>
+      <c r="H12" s="75"/>
       <c r="I12" s="14" t="s">
         <v>11</v>
       </c>
       <c r="J12" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="K12" s="109" t="s">
+      <c r="K12" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="L12" s="110"/>
-      <c r="M12" s="110"/>
-      <c r="N12" s="110"/>
+      <c r="L12" s="74"/>
+      <c r="M12" s="74"/>
+      <c r="N12" s="74"/>
       <c r="O12" s="15" t="s">
         <v>11</v>
       </c>
       <c r="P12" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="Q12" s="109" t="s">
+      <c r="Q12" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="R12" s="110"/>
-      <c r="S12" s="110"/>
-      <c r="T12" s="111"/>
+      <c r="R12" s="74"/>
+      <c r="S12" s="74"/>
+      <c r="T12" s="75"/>
       <c r="U12" s="63" t="s">
         <v>11</v>
       </c>
       <c r="V12" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="W12" s="109" t="s">
+      <c r="W12" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="X12" s="110"/>
-      <c r="Y12" s="110"/>
-      <c r="Z12" s="111"/>
+      <c r="X12" s="74"/>
+      <c r="Y12" s="74"/>
+      <c r="Z12" s="75"/>
     </row>
     <row r="13" spans="2:26" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="55"/>
@@ -4430,20 +4430,20 @@
     </row>
     <row r="37" spans="2:26" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B37" s="59"/>
-      <c r="C37" s="112" t="s">
+      <c r="C37" s="106" t="s">
         <v>33</v>
       </c>
-      <c r="D37" s="113"/>
+      <c r="D37" s="107"/>
       <c r="E37" s="60"/>
       <c r="F37" s="60"/>
       <c r="G37" s="61" t="s">
         <v>31</v>
       </c>
       <c r="H37" s="60"/>
-      <c r="I37" s="112" t="s">
+      <c r="I37" s="106" t="s">
         <v>33</v>
       </c>
-      <c r="J37" s="114">
+      <c r="J37" s="108">
         <v>20</v>
       </c>
       <c r="K37" s="60"/>
@@ -4452,10 +4452,10 @@
         <v>31</v>
       </c>
       <c r="N37" s="60"/>
-      <c r="O37" s="112" t="s">
+      <c r="O37" s="106" t="s">
         <v>33</v>
       </c>
-      <c r="P37" s="114">
+      <c r="P37" s="108">
         <v>20</v>
       </c>
       <c r="Q37" s="60"/>
@@ -4464,10 +4464,10 @@
         <v>31</v>
       </c>
       <c r="T37" s="60"/>
-      <c r="U37" s="112" t="s">
+      <c r="U37" s="106" t="s">
         <v>33</v>
       </c>
-      <c r="V37" s="115"/>
+      <c r="V37" s="109"/>
       <c r="W37" s="60"/>
       <c r="X37" s="60"/>
       <c r="Y37" s="61" t="s">
@@ -4476,270 +4476,267 @@
       <c r="Z37" s="62"/>
     </row>
     <row r="38" spans="2:26" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="100" t="s">
+      <c r="B38" s="97" t="s">
         <v>68</v>
       </c>
-      <c r="C38" s="101"/>
-      <c r="D38" s="101"/>
-      <c r="E38" s="101"/>
-      <c r="F38" s="101"/>
-      <c r="G38" s="101"/>
-      <c r="H38" s="101"/>
-      <c r="I38" s="101"/>
-      <c r="J38" s="101"/>
-      <c r="K38" s="101"/>
-      <c r="L38" s="101"/>
-      <c r="M38" s="101"/>
-      <c r="N38" s="101"/>
-      <c r="O38" s="101"/>
-      <c r="P38" s="101"/>
-      <c r="Q38" s="101"/>
-      <c r="R38" s="101"/>
-      <c r="S38" s="101"/>
-      <c r="T38" s="101"/>
-      <c r="U38" s="101"/>
-      <c r="V38" s="101"/>
-      <c r="W38" s="101"/>
-      <c r="X38" s="101"/>
-      <c r="Y38" s="101"/>
-      <c r="Z38" s="102"/>
+      <c r="C38" s="98"/>
+      <c r="D38" s="98"/>
+      <c r="E38" s="98"/>
+      <c r="F38" s="98"/>
+      <c r="G38" s="98"/>
+      <c r="H38" s="98"/>
+      <c r="I38" s="98"/>
+      <c r="J38" s="98"/>
+      <c r="K38" s="98"/>
+      <c r="L38" s="98"/>
+      <c r="M38" s="98"/>
+      <c r="N38" s="98"/>
+      <c r="O38" s="98"/>
+      <c r="P38" s="98"/>
+      <c r="Q38" s="98"/>
+      <c r="R38" s="98"/>
+      <c r="S38" s="98"/>
+      <c r="T38" s="98"/>
+      <c r="U38" s="98"/>
+      <c r="V38" s="98"/>
+      <c r="W38" s="98"/>
+      <c r="X38" s="98"/>
+      <c r="Y38" s="98"/>
+      <c r="Z38" s="99"/>
     </row>
     <row r="39" spans="2:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="103" t="s">
+      <c r="B39" s="100" t="s">
         <v>34</v>
       </c>
-      <c r="C39" s="104"/>
-      <c r="D39" s="104"/>
-      <c r="E39" s="104"/>
-      <c r="F39" s="104"/>
-      <c r="G39" s="104"/>
-      <c r="H39" s="104"/>
-      <c r="I39" s="104"/>
-      <c r="J39" s="104"/>
-      <c r="K39" s="104"/>
-      <c r="L39" s="104"/>
-      <c r="M39" s="104"/>
-      <c r="N39" s="104"/>
-      <c r="O39" s="104"/>
-      <c r="P39" s="104"/>
-      <c r="Q39" s="104"/>
-      <c r="R39" s="104"/>
-      <c r="S39" s="104"/>
-      <c r="T39" s="104"/>
-      <c r="U39" s="104"/>
-      <c r="V39" s="104"/>
-      <c r="W39" s="104"/>
-      <c r="X39" s="104"/>
-      <c r="Y39" s="104"/>
-      <c r="Z39" s="105"/>
+      <c r="C39" s="101"/>
+      <c r="D39" s="101"/>
+      <c r="E39" s="101"/>
+      <c r="F39" s="101"/>
+      <c r="G39" s="101"/>
+      <c r="H39" s="101"/>
+      <c r="I39" s="101"/>
+      <c r="J39" s="101"/>
+      <c r="K39" s="101"/>
+      <c r="L39" s="101"/>
+      <c r="M39" s="101"/>
+      <c r="N39" s="101"/>
+      <c r="O39" s="101"/>
+      <c r="P39" s="101"/>
+      <c r="Q39" s="101"/>
+      <c r="R39" s="101"/>
+      <c r="S39" s="101"/>
+      <c r="T39" s="101"/>
+      <c r="U39" s="101"/>
+      <c r="V39" s="101"/>
+      <c r="W39" s="101"/>
+      <c r="X39" s="101"/>
+      <c r="Y39" s="101"/>
+      <c r="Z39" s="102"/>
     </row>
     <row r="40" spans="2:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="106"/>
-      <c r="C40" s="107"/>
-      <c r="D40" s="107"/>
-      <c r="E40" s="107"/>
-      <c r="F40" s="107"/>
-      <c r="G40" s="107"/>
-      <c r="H40" s="107"/>
-      <c r="I40" s="107"/>
-      <c r="J40" s="107"/>
-      <c r="K40" s="107"/>
-      <c r="L40" s="107"/>
-      <c r="M40" s="107"/>
-      <c r="N40" s="107"/>
-      <c r="O40" s="107"/>
-      <c r="P40" s="107"/>
-      <c r="Q40" s="107"/>
-      <c r="R40" s="107"/>
-      <c r="S40" s="107"/>
-      <c r="T40" s="107"/>
-      <c r="U40" s="107"/>
-      <c r="V40" s="107"/>
-      <c r="W40" s="107"/>
-      <c r="X40" s="107"/>
-      <c r="Y40" s="107"/>
-      <c r="Z40" s="108"/>
+      <c r="B40" s="103"/>
+      <c r="C40" s="104"/>
+      <c r="D40" s="104"/>
+      <c r="E40" s="104"/>
+      <c r="F40" s="104"/>
+      <c r="G40" s="104"/>
+      <c r="H40" s="104"/>
+      <c r="I40" s="104"/>
+      <c r="J40" s="104"/>
+      <c r="K40" s="104"/>
+      <c r="L40" s="104"/>
+      <c r="M40" s="104"/>
+      <c r="N40" s="104"/>
+      <c r="O40" s="104"/>
+      <c r="P40" s="104"/>
+      <c r="Q40" s="104"/>
+      <c r="R40" s="104"/>
+      <c r="S40" s="104"/>
+      <c r="T40" s="104"/>
+      <c r="U40" s="104"/>
+      <c r="V40" s="104"/>
+      <c r="W40" s="104"/>
+      <c r="X40" s="104"/>
+      <c r="Y40" s="104"/>
+      <c r="Z40" s="105"/>
     </row>
     <row r="41" spans="2:26" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="122"/>
-      <c r="C41" s="123"/>
-      <c r="D41" s="123"/>
-      <c r="E41" s="123"/>
-      <c r="F41" s="123"/>
-      <c r="G41" s="123"/>
-      <c r="H41" s="123"/>
-      <c r="I41" s="123"/>
-      <c r="J41" s="123"/>
-      <c r="K41" s="123"/>
-      <c r="L41" s="123"/>
-      <c r="M41" s="123"/>
-      <c r="N41" s="123"/>
-      <c r="O41" s="123"/>
-      <c r="P41" s="123"/>
-      <c r="Q41" s="123"/>
-      <c r="R41" s="123"/>
-      <c r="S41" s="123"/>
-      <c r="T41" s="123"/>
-      <c r="U41" s="123"/>
-      <c r="V41" s="123"/>
-      <c r="W41" s="123"/>
-      <c r="X41" s="123"/>
-      <c r="Y41" s="123"/>
-      <c r="Z41" s="124"/>
+      <c r="B41" s="82"/>
+      <c r="C41" s="83"/>
+      <c r="D41" s="83"/>
+      <c r="E41" s="83"/>
+      <c r="F41" s="83"/>
+      <c r="G41" s="83"/>
+      <c r="H41" s="83"/>
+      <c r="I41" s="83"/>
+      <c r="J41" s="83"/>
+      <c r="K41" s="83"/>
+      <c r="L41" s="83"/>
+      <c r="M41" s="83"/>
+      <c r="N41" s="83"/>
+      <c r="O41" s="83"/>
+      <c r="P41" s="83"/>
+      <c r="Q41" s="83"/>
+      <c r="R41" s="83"/>
+      <c r="S41" s="83"/>
+      <c r="T41" s="83"/>
+      <c r="U41" s="83"/>
+      <c r="V41" s="83"/>
+      <c r="W41" s="83"/>
+      <c r="X41" s="83"/>
+      <c r="Y41" s="83"/>
+      <c r="Z41" s="84"/>
     </row>
     <row r="42" spans="2:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="125" t="s">
+      <c r="B42" s="85" t="s">
         <v>35</v>
       </c>
-      <c r="C42" s="126"/>
-      <c r="D42" s="126"/>
-      <c r="E42" s="126"/>
-      <c r="F42" s="126"/>
-      <c r="G42" s="126"/>
-      <c r="H42" s="126"/>
-      <c r="I42" s="127"/>
-      <c r="J42" s="128" t="s">
+      <c r="C42" s="86"/>
+      <c r="D42" s="86"/>
+      <c r="E42" s="86"/>
+      <c r="F42" s="86"/>
+      <c r="G42" s="86"/>
+      <c r="H42" s="86"/>
+      <c r="I42" s="87"/>
+      <c r="J42" s="88" t="s">
         <v>36</v>
       </c>
-      <c r="K42" s="129"/>
-      <c r="L42" s="129"/>
-      <c r="M42" s="129"/>
-      <c r="N42" s="129"/>
-      <c r="O42" s="129"/>
-      <c r="P42" s="129"/>
-      <c r="Q42" s="129"/>
-      <c r="R42" s="130"/>
-      <c r="S42" s="128" t="s">
+      <c r="K42" s="89"/>
+      <c r="L42" s="89"/>
+      <c r="M42" s="89"/>
+      <c r="N42" s="89"/>
+      <c r="O42" s="89"/>
+      <c r="P42" s="89"/>
+      <c r="Q42" s="89"/>
+      <c r="R42" s="90"/>
+      <c r="S42" s="88" t="s">
         <v>41</v>
       </c>
-      <c r="T42" s="129"/>
-      <c r="U42" s="129"/>
-      <c r="V42" s="129"/>
-      <c r="W42" s="129"/>
-      <c r="X42" s="129"/>
-      <c r="Y42" s="129"/>
-      <c r="Z42" s="130"/>
+      <c r="T42" s="89"/>
+      <c r="U42" s="89"/>
+      <c r="V42" s="89"/>
+      <c r="W42" s="89"/>
+      <c r="X42" s="89"/>
+      <c r="Y42" s="89"/>
+      <c r="Z42" s="90"/>
     </row>
     <row r="43" spans="2:26" s="54" customFormat="1" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="94" t="s">
+      <c r="B43" s="91" t="s">
         <v>37</v>
       </c>
-      <c r="C43" s="95"/>
-      <c r="D43" s="95"/>
-      <c r="E43" s="95"/>
-      <c r="F43" s="95"/>
-      <c r="G43" s="95"/>
-      <c r="H43" s="95"/>
-      <c r="I43" s="96"/>
-      <c r="J43" s="97" t="s">
+      <c r="C43" s="92"/>
+      <c r="D43" s="92"/>
+      <c r="E43" s="92"/>
+      <c r="F43" s="92"/>
+      <c r="G43" s="92"/>
+      <c r="H43" s="92"/>
+      <c r="I43" s="93"/>
+      <c r="J43" s="94" t="s">
         <v>14</v>
       </c>
-      <c r="K43" s="98"/>
-      <c r="L43" s="98"/>
-      <c r="M43" s="98"/>
-      <c r="N43" s="98"/>
-      <c r="O43" s="98"/>
-      <c r="P43" s="98"/>
-      <c r="Q43" s="98"/>
-      <c r="R43" s="99"/>
-      <c r="S43" s="97" t="s">
+      <c r="K43" s="95"/>
+      <c r="L43" s="95"/>
+      <c r="M43" s="95"/>
+      <c r="N43" s="95"/>
+      <c r="O43" s="95"/>
+      <c r="P43" s="95"/>
+      <c r="Q43" s="95"/>
+      <c r="R43" s="96"/>
+      <c r="S43" s="94" t="s">
         <v>14</v>
       </c>
-      <c r="T43" s="98"/>
-      <c r="U43" s="98"/>
-      <c r="V43" s="98"/>
-      <c r="W43" s="98"/>
-      <c r="X43" s="98"/>
-      <c r="Y43" s="98"/>
-      <c r="Z43" s="99"/>
+      <c r="T43" s="95"/>
+      <c r="U43" s="95"/>
+      <c r="V43" s="95"/>
+      <c r="W43" s="95"/>
+      <c r="X43" s="95"/>
+      <c r="Y43" s="95"/>
+      <c r="Z43" s="96"/>
     </row>
     <row r="44" spans="2:26" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="94" t="s">
+      <c r="B44" s="91" t="s">
         <v>55</v>
       </c>
-      <c r="C44" s="95"/>
-      <c r="D44" s="95"/>
-      <c r="E44" s="95"/>
-      <c r="F44" s="95"/>
-      <c r="G44" s="95"/>
-      <c r="H44" s="95"/>
-      <c r="I44" s="96"/>
-      <c r="J44" s="97" t="s">
+      <c r="C44" s="92"/>
+      <c r="D44" s="92"/>
+      <c r="E44" s="92"/>
+      <c r="F44" s="92"/>
+      <c r="G44" s="92"/>
+      <c r="H44" s="92"/>
+      <c r="I44" s="93"/>
+      <c r="J44" s="94" t="s">
         <v>56</v>
       </c>
-      <c r="K44" s="98"/>
-      <c r="L44" s="98"/>
-      <c r="M44" s="98"/>
-      <c r="N44" s="98"/>
-      <c r="O44" s="98"/>
-      <c r="P44" s="98"/>
-      <c r="Q44" s="98"/>
-      <c r="R44" s="99"/>
-      <c r="S44" s="97" t="s">
+      <c r="K44" s="95"/>
+      <c r="L44" s="95"/>
+      <c r="M44" s="95"/>
+      <c r="N44" s="95"/>
+      <c r="O44" s="95"/>
+      <c r="P44" s="95"/>
+      <c r="Q44" s="95"/>
+      <c r="R44" s="96"/>
+      <c r="S44" s="94" t="s">
         <v>56</v>
       </c>
-      <c r="T44" s="98"/>
-      <c r="U44" s="98"/>
-      <c r="V44" s="98"/>
-      <c r="W44" s="98"/>
-      <c r="X44" s="98"/>
-      <c r="Y44" s="98"/>
-      <c r="Z44" s="99"/>
+      <c r="T44" s="95"/>
+      <c r="U44" s="95"/>
+      <c r="V44" s="95"/>
+      <c r="W44" s="95"/>
+      <c r="X44" s="95"/>
+      <c r="Y44" s="95"/>
+      <c r="Z44" s="96"/>
     </row>
     <row r="45" spans="2:26" ht="87.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="116" t="s">
+      <c r="B45" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="C45" s="117"/>
-      <c r="D45" s="117"/>
-      <c r="E45" s="117"/>
-      <c r="F45" s="117"/>
-      <c r="G45" s="117"/>
-      <c r="H45" s="117"/>
-      <c r="I45" s="118"/>
-      <c r="J45" s="119" t="s">
+      <c r="C45" s="77"/>
+      <c r="D45" s="77"/>
+      <c r="E45" s="77"/>
+      <c r="F45" s="77"/>
+      <c r="G45" s="77"/>
+      <c r="H45" s="77"/>
+      <c r="I45" s="78"/>
+      <c r="J45" s="79" t="s">
         <v>38</v>
       </c>
-      <c r="K45" s="120"/>
-      <c r="L45" s="120"/>
-      <c r="M45" s="120"/>
-      <c r="N45" s="120"/>
-      <c r="O45" s="120"/>
-      <c r="P45" s="120"/>
-      <c r="Q45" s="120"/>
-      <c r="R45" s="121"/>
-      <c r="S45" s="119" t="s">
+      <c r="K45" s="80"/>
+      <c r="L45" s="80"/>
+      <c r="M45" s="80"/>
+      <c r="N45" s="80"/>
+      <c r="O45" s="80"/>
+      <c r="P45" s="80"/>
+      <c r="Q45" s="80"/>
+      <c r="R45" s="81"/>
+      <c r="S45" s="79" t="s">
         <v>67</v>
       </c>
-      <c r="T45" s="120"/>
-      <c r="U45" s="120"/>
-      <c r="V45" s="120"/>
-      <c r="W45" s="120"/>
-      <c r="X45" s="120"/>
-      <c r="Y45" s="120"/>
-      <c r="Z45" s="121"/>
+      <c r="T45" s="80"/>
+      <c r="U45" s="80"/>
+      <c r="V45" s="80"/>
+      <c r="W45" s="80"/>
+      <c r="X45" s="80"/>
+      <c r="Y45" s="80"/>
+      <c r="Z45" s="81"/>
     </row>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="C11:H11"/>
-    <mergeCell ref="I11:N11"/>
-    <mergeCell ref="O11:T11"/>
-    <mergeCell ref="U11:Z11"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="C10:H10"/>
-    <mergeCell ref="I10:N10"/>
-    <mergeCell ref="E12:H12"/>
-    <mergeCell ref="K12:N12"/>
-    <mergeCell ref="B45:I45"/>
-    <mergeCell ref="J45:R45"/>
-    <mergeCell ref="S45:Z45"/>
-    <mergeCell ref="B41:Z41"/>
-    <mergeCell ref="B42:I42"/>
-    <mergeCell ref="J42:R42"/>
-    <mergeCell ref="S42:Z42"/>
-    <mergeCell ref="B43:I43"/>
-    <mergeCell ref="J43:R43"/>
-    <mergeCell ref="S43:Z43"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="G9:N9"/>
+    <mergeCell ref="O9:S9"/>
+    <mergeCell ref="T9:Z9"/>
+    <mergeCell ref="B2:Z3"/>
+    <mergeCell ref="Q6:Z6"/>
+    <mergeCell ref="J6:P6"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="X4:Z4"/>
+    <mergeCell ref="X5:Z5"/>
+    <mergeCell ref="B4:W5"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="J7:P7"/>
+    <mergeCell ref="Q7:Z7"/>
+    <mergeCell ref="T8:Z8"/>
+    <mergeCell ref="O8:S8"/>
     <mergeCell ref="B8:F8"/>
     <mergeCell ref="G8:N8"/>
     <mergeCell ref="B44:I44"/>
@@ -4756,22 +4753,25 @@
     <mergeCell ref="U37:V37"/>
     <mergeCell ref="O10:T10"/>
     <mergeCell ref="U10:Z10"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="G9:N9"/>
-    <mergeCell ref="O9:S9"/>
-    <mergeCell ref="T9:Z9"/>
-    <mergeCell ref="B2:Z3"/>
-    <mergeCell ref="Q6:Z6"/>
-    <mergeCell ref="J6:P6"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="X4:Z4"/>
-    <mergeCell ref="X5:Z5"/>
-    <mergeCell ref="B4:W5"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="J7:P7"/>
-    <mergeCell ref="Q7:Z7"/>
-    <mergeCell ref="T8:Z8"/>
-    <mergeCell ref="O8:S8"/>
+    <mergeCell ref="B45:I45"/>
+    <mergeCell ref="J45:R45"/>
+    <mergeCell ref="S45:Z45"/>
+    <mergeCell ref="B41:Z41"/>
+    <mergeCell ref="B42:I42"/>
+    <mergeCell ref="J42:R42"/>
+    <mergeCell ref="S42:Z42"/>
+    <mergeCell ref="B43:I43"/>
+    <mergeCell ref="J43:R43"/>
+    <mergeCell ref="S43:Z43"/>
+    <mergeCell ref="C11:H11"/>
+    <mergeCell ref="I11:N11"/>
+    <mergeCell ref="O11:T11"/>
+    <mergeCell ref="U11:Z11"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="I10:N10"/>
+    <mergeCell ref="E12:H12"/>
+    <mergeCell ref="K12:N12"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.19685039370078741" top="0.74803149606299213" bottom="0.74803149606299213" header="0.98425196850393704" footer="0.31496062992125984"/>
@@ -4803,16 +4803,16 @@
   <sheetData>
     <row r="1" spans="2:17" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:17" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="150"/>
-      <c r="C2" s="150"/>
-      <c r="D2" s="150"/>
-      <c r="E2" s="150"/>
-      <c r="F2" s="150"/>
-      <c r="G2" s="150"/>
-      <c r="H2" s="150"/>
-      <c r="I2" s="150"/>
-      <c r="J2" s="150"/>
-      <c r="K2" s="150"/>
+      <c r="B2" s="126"/>
+      <c r="C2" s="126"/>
+      <c r="D2" s="126"/>
+      <c r="E2" s="126"/>
+      <c r="F2" s="126"/>
+      <c r="G2" s="126"/>
+      <c r="H2" s="126"/>
+      <c r="I2" s="126"/>
+      <c r="J2" s="126"/>
+      <c r="K2" s="126"/>
       <c r="L2" s="5"/>
       <c r="M2" s="6"/>
       <c r="N2" s="6"/>
@@ -4820,16 +4820,16 @@
       <c r="P2" s="6"/>
     </row>
     <row r="3" spans="2:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="150"/>
-      <c r="C3" s="150"/>
-      <c r="D3" s="150"/>
-      <c r="E3" s="150"/>
-      <c r="F3" s="150"/>
-      <c r="G3" s="150"/>
-      <c r="H3" s="150"/>
-      <c r="I3" s="150"/>
-      <c r="J3" s="150"/>
-      <c r="K3" s="150"/>
+      <c r="B3" s="126"/>
+      <c r="C3" s="126"/>
+      <c r="D3" s="126"/>
+      <c r="E3" s="126"/>
+      <c r="F3" s="126"/>
+      <c r="G3" s="126"/>
+      <c r="H3" s="126"/>
+      <c r="I3" s="126"/>
+      <c r="J3" s="126"/>
+      <c r="K3" s="126"/>
       <c r="L3" s="5"/>
       <c r="M3" s="6"/>
       <c r="N3" s="6"/>
@@ -4837,17 +4837,17 @@
       <c r="P3" s="6"/>
     </row>
     <row r="4" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="83" t="s">
+      <c r="B4" s="121" t="s">
         <v>66</v>
       </c>
-      <c r="C4" s="83"/>
-      <c r="D4" s="83"/>
-      <c r="E4" s="83"/>
-      <c r="F4" s="83"/>
-      <c r="G4" s="83"/>
-      <c r="H4" s="83"/>
-      <c r="I4" s="83"/>
-      <c r="J4" s="83"/>
+      <c r="C4" s="121"/>
+      <c r="D4" s="121"/>
+      <c r="E4" s="121"/>
+      <c r="F4" s="121"/>
+      <c r="G4" s="121"/>
+      <c r="H4" s="121"/>
+      <c r="I4" s="121"/>
+      <c r="J4" s="121"/>
       <c r="K4" s="8" t="s">
         <v>65</v>
       </c>
@@ -4858,15 +4858,15 @@
       <c r="P4" s="6"/>
     </row>
     <row r="5" spans="2:17" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="83"/>
-      <c r="C5" s="83"/>
-      <c r="D5" s="83"/>
-      <c r="E5" s="83"/>
-      <c r="F5" s="83"/>
-      <c r="G5" s="83"/>
-      <c r="H5" s="83"/>
-      <c r="I5" s="83"/>
-      <c r="J5" s="83"/>
+      <c r="B5" s="121"/>
+      <c r="C5" s="121"/>
+      <c r="D5" s="121"/>
+      <c r="E5" s="121"/>
+      <c r="F5" s="121"/>
+      <c r="G5" s="121"/>
+      <c r="H5" s="121"/>
+      <c r="I5" s="121"/>
+      <c r="J5" s="121"/>
       <c r="K5" s="7" t="s">
         <v>63</v>
       </c>
@@ -4878,397 +4878,373 @@
       <c r="Q5" s="1"/>
     </row>
     <row r="6" spans="2:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="151" t="s">
+      <c r="B6" s="127" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="151"/>
-      <c r="D6" s="151"/>
-      <c r="E6" s="151"/>
-      <c r="F6" s="151"/>
-      <c r="G6" s="151"/>
-      <c r="H6" s="151"/>
-      <c r="I6" s="151"/>
-      <c r="J6" s="151"/>
-      <c r="K6" s="151"/>
+      <c r="C6" s="127"/>
+      <c r="D6" s="127"/>
+      <c r="E6" s="127"/>
+      <c r="F6" s="127"/>
+      <c r="G6" s="127"/>
+      <c r="H6" s="127"/>
+      <c r="I6" s="127"/>
+      <c r="J6" s="127"/>
+      <c r="K6" s="127"/>
     </row>
     <row r="7" spans="2:17" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B7" s="152" t="s">
+      <c r="B7" s="128" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="152"/>
-      <c r="D7" s="152"/>
-      <c r="E7" s="152"/>
-      <c r="F7" s="152"/>
-      <c r="G7" s="152"/>
-      <c r="H7" s="152"/>
-      <c r="I7" s="152"/>
-      <c r="J7" s="152"/>
-      <c r="K7" s="152"/>
+      <c r="C7" s="128"/>
+      <c r="D7" s="128"/>
+      <c r="E7" s="128"/>
+      <c r="F7" s="128"/>
+      <c r="G7" s="128"/>
+      <c r="H7" s="128"/>
+      <c r="I7" s="128"/>
+      <c r="J7" s="128"/>
+      <c r="K7" s="128"/>
     </row>
     <row r="8" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B8" s="153" t="s">
+      <c r="B8" s="124" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="153"/>
-      <c r="D8" s="153"/>
-      <c r="E8" s="153"/>
-      <c r="F8" s="153"/>
-      <c r="G8" s="153"/>
-      <c r="H8" s="153"/>
-      <c r="I8" s="153"/>
-      <c r="J8" s="153"/>
-      <c r="K8" s="153"/>
+      <c r="C8" s="124"/>
+      <c r="D8" s="124"/>
+      <c r="E8" s="124"/>
+      <c r="F8" s="124"/>
+      <c r="G8" s="124"/>
+      <c r="H8" s="124"/>
+      <c r="I8" s="124"/>
+      <c r="J8" s="124"/>
+      <c r="K8" s="124"/>
     </row>
     <row r="9" spans="2:17" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="154" t="s">
+      <c r="B9" s="125" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="154"/>
-      <c r="D9" s="154"/>
-      <c r="E9" s="154"/>
-      <c r="F9" s="154"/>
-      <c r="G9" s="154"/>
-      <c r="H9" s="154"/>
-      <c r="I9" s="154"/>
-      <c r="J9" s="154"/>
-      <c r="K9" s="154"/>
+      <c r="C9" s="125"/>
+      <c r="D9" s="125"/>
+      <c r="E9" s="125"/>
+      <c r="F9" s="125"/>
+      <c r="G9" s="125"/>
+      <c r="H9" s="125"/>
+      <c r="I9" s="125"/>
+      <c r="J9" s="125"/>
+      <c r="K9" s="125"/>
     </row>
     <row r="10" spans="2:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="154" t="s">
+      <c r="B10" s="125" t="s">
         <v>58</v>
       </c>
-      <c r="C10" s="154"/>
-      <c r="D10" s="154"/>
-      <c r="E10" s="154"/>
-      <c r="F10" s="154"/>
-      <c r="G10" s="154"/>
-      <c r="H10" s="154"/>
-      <c r="I10" s="154"/>
-      <c r="J10" s="154"/>
-      <c r="K10" s="154"/>
+      <c r="C10" s="125"/>
+      <c r="D10" s="125"/>
+      <c r="E10" s="125"/>
+      <c r="F10" s="125"/>
+      <c r="G10" s="125"/>
+      <c r="H10" s="125"/>
+      <c r="I10" s="125"/>
+      <c r="J10" s="125"/>
+      <c r="K10" s="125"/>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B11" s="154" t="s">
+      <c r="B11" s="125" t="s">
         <v>59</v>
       </c>
-      <c r="C11" s="154"/>
-      <c r="D11" s="154"/>
-      <c r="E11" s="154"/>
-      <c r="F11" s="154"/>
-      <c r="G11" s="154"/>
-      <c r="H11" s="154"/>
-      <c r="I11" s="154"/>
-      <c r="J11" s="154"/>
-      <c r="K11" s="154"/>
+      <c r="C11" s="125"/>
+      <c r="D11" s="125"/>
+      <c r="E11" s="125"/>
+      <c r="F11" s="125"/>
+      <c r="G11" s="125"/>
+      <c r="H11" s="125"/>
+      <c r="I11" s="125"/>
+      <c r="J11" s="125"/>
+      <c r="K11" s="125"/>
     </row>
     <row r="12" spans="2:17" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="154" t="s">
+      <c r="B12" s="125" t="s">
         <v>61</v>
       </c>
-      <c r="C12" s="154"/>
-      <c r="D12" s="154"/>
-      <c r="E12" s="154"/>
-      <c r="F12" s="154"/>
-      <c r="G12" s="154"/>
-      <c r="H12" s="154"/>
-      <c r="I12" s="154"/>
-      <c r="J12" s="154"/>
-      <c r="K12" s="154"/>
+      <c r="C12" s="125"/>
+      <c r="D12" s="125"/>
+      <c r="E12" s="125"/>
+      <c r="F12" s="125"/>
+      <c r="G12" s="125"/>
+      <c r="H12" s="125"/>
+      <c r="I12" s="125"/>
+      <c r="J12" s="125"/>
+      <c r="K12" s="125"/>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B13" s="154" t="s">
+      <c r="B13" s="125" t="s">
         <v>60</v>
       </c>
-      <c r="C13" s="154"/>
-      <c r="D13" s="154"/>
-      <c r="E13" s="154"/>
-      <c r="F13" s="154"/>
-      <c r="G13" s="154"/>
-      <c r="H13" s="154"/>
-      <c r="I13" s="154"/>
-      <c r="J13" s="154"/>
-      <c r="K13" s="154"/>
+      <c r="C13" s="125"/>
+      <c r="D13" s="125"/>
+      <c r="E13" s="125"/>
+      <c r="F13" s="125"/>
+      <c r="G13" s="125"/>
+      <c r="H13" s="125"/>
+      <c r="I13" s="125"/>
+      <c r="J13" s="125"/>
+      <c r="K13" s="125"/>
     </row>
     <row r="14" spans="2:17" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="154" t="s">
+      <c r="B14" s="125" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="154"/>
-      <c r="D14" s="154"/>
-      <c r="E14" s="154"/>
-      <c r="F14" s="154"/>
-      <c r="G14" s="154"/>
-      <c r="H14" s="154"/>
-      <c r="I14" s="154"/>
-      <c r="J14" s="154"/>
-      <c r="K14" s="154"/>
+      <c r="C14" s="125"/>
+      <c r="D14" s="125"/>
+      <c r="E14" s="125"/>
+      <c r="F14" s="125"/>
+      <c r="G14" s="125"/>
+      <c r="H14" s="125"/>
+      <c r="I14" s="125"/>
+      <c r="J14" s="125"/>
+      <c r="K14" s="125"/>
     </row>
     <row r="15" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B15" s="153" t="s">
+      <c r="B15" s="124" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="153"/>
-      <c r="D15" s="153"/>
-      <c r="E15" s="153"/>
-      <c r="F15" s="153"/>
-      <c r="G15" s="153"/>
-      <c r="H15" s="153"/>
-      <c r="I15" s="153"/>
-      <c r="J15" s="153"/>
-      <c r="K15" s="153"/>
+      <c r="C15" s="124"/>
+      <c r="D15" s="124"/>
+      <c r="E15" s="124"/>
+      <c r="F15" s="124"/>
+      <c r="G15" s="124"/>
+      <c r="H15" s="124"/>
+      <c r="I15" s="124"/>
+      <c r="J15" s="124"/>
+      <c r="K15" s="124"/>
     </row>
     <row r="16" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="142" t="s">
+      <c r="C16" s="137" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="142"/>
-      <c r="E16" s="142"/>
-      <c r="F16" s="142"/>
-      <c r="G16" s="142"/>
-      <c r="H16" s="142" t="s">
+      <c r="D16" s="137"/>
+      <c r="E16" s="137"/>
+      <c r="F16" s="137"/>
+      <c r="G16" s="137"/>
+      <c r="H16" s="137" t="s">
         <v>6</v>
       </c>
-      <c r="I16" s="142"/>
-      <c r="J16" s="142"/>
-      <c r="K16" s="142"/>
+      <c r="I16" s="137"/>
+      <c r="J16" s="137"/>
+      <c r="K16" s="137"/>
     </row>
     <row r="17" spans="2:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="140" t="s">
+      <c r="C17" s="133" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="140"/>
-      <c r="E17" s="140"/>
-      <c r="F17" s="140"/>
-      <c r="G17" s="140"/>
-      <c r="H17" s="141"/>
-      <c r="I17" s="141"/>
-      <c r="J17" s="141"/>
-      <c r="K17" s="141"/>
+      <c r="D17" s="133"/>
+      <c r="E17" s="133"/>
+      <c r="F17" s="133"/>
+      <c r="G17" s="133"/>
+      <c r="H17" s="132"/>
+      <c r="I17" s="132"/>
+      <c r="J17" s="132"/>
+      <c r="K17" s="132"/>
     </row>
     <row r="18" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="140" t="s">
+      <c r="C18" s="133" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="140"/>
-      <c r="E18" s="140"/>
-      <c r="F18" s="140"/>
-      <c r="G18" s="140"/>
-      <c r="H18" s="141"/>
-      <c r="I18" s="141"/>
-      <c r="J18" s="141"/>
-      <c r="K18" s="141"/>
+      <c r="D18" s="133"/>
+      <c r="E18" s="133"/>
+      <c r="F18" s="133"/>
+      <c r="G18" s="133"/>
+      <c r="H18" s="132"/>
+      <c r="I18" s="132"/>
+      <c r="J18" s="132"/>
+      <c r="K18" s="132"/>
     </row>
     <row r="19" spans="2:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="140" t="s">
+      <c r="C19" s="133" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="140"/>
-      <c r="E19" s="140"/>
-      <c r="F19" s="140"/>
-      <c r="G19" s="140"/>
-      <c r="H19" s="141"/>
-      <c r="I19" s="141"/>
-      <c r="J19" s="141"/>
-      <c r="K19" s="141"/>
+      <c r="D19" s="133"/>
+      <c r="E19" s="133"/>
+      <c r="F19" s="133"/>
+      <c r="G19" s="133"/>
+      <c r="H19" s="132"/>
+      <c r="I19" s="132"/>
+      <c r="J19" s="132"/>
+      <c r="K19" s="132"/>
     </row>
     <row r="20" spans="2:11" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="143" t="s">
+      <c r="C20" s="138" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="143"/>
-      <c r="E20" s="143"/>
-      <c r="F20" s="143"/>
-      <c r="G20" s="143"/>
-      <c r="H20" s="141"/>
-      <c r="I20" s="141"/>
-      <c r="J20" s="141"/>
-      <c r="K20" s="141"/>
+      <c r="D20" s="138"/>
+      <c r="E20" s="138"/>
+      <c r="F20" s="138"/>
+      <c r="G20" s="138"/>
+      <c r="H20" s="132"/>
+      <c r="I20" s="132"/>
+      <c r="J20" s="132"/>
+      <c r="K20" s="132"/>
     </row>
     <row r="21" spans="2:11" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="140" t="s">
+      <c r="C21" s="133" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="140"/>
-      <c r="E21" s="140"/>
-      <c r="F21" s="140"/>
-      <c r="G21" s="140"/>
-      <c r="H21" s="141"/>
-      <c r="I21" s="141"/>
-      <c r="J21" s="141"/>
-      <c r="K21" s="141"/>
+      <c r="D21" s="133"/>
+      <c r="E21" s="133"/>
+      <c r="F21" s="133"/>
+      <c r="G21" s="133"/>
+      <c r="H21" s="132"/>
+      <c r="I21" s="132"/>
+      <c r="J21" s="132"/>
+      <c r="K21" s="132"/>
     </row>
     <row r="22" spans="2:11" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="140" t="s">
+      <c r="C22" s="133" t="s">
         <v>42</v>
       </c>
-      <c r="D22" s="140"/>
-      <c r="E22" s="140"/>
-      <c r="F22" s="140"/>
-      <c r="G22" s="140"/>
-      <c r="H22" s="141"/>
-      <c r="I22" s="141"/>
-      <c r="J22" s="141"/>
-      <c r="K22" s="141"/>
+      <c r="D22" s="133"/>
+      <c r="E22" s="133"/>
+      <c r="F22" s="133"/>
+      <c r="G22" s="133"/>
+      <c r="H22" s="132"/>
+      <c r="I22" s="132"/>
+      <c r="J22" s="132"/>
+      <c r="K22" s="132"/>
     </row>
     <row r="23" spans="2:11" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="140" t="s">
+      <c r="C23" s="133" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="140"/>
-      <c r="E23" s="140"/>
-      <c r="F23" s="140"/>
-      <c r="G23" s="140"/>
-      <c r="H23" s="141"/>
-      <c r="I23" s="141"/>
-      <c r="J23" s="141"/>
-      <c r="K23" s="141"/>
+      <c r="D23" s="133"/>
+      <c r="E23" s="133"/>
+      <c r="F23" s="133"/>
+      <c r="G23" s="133"/>
+      <c r="H23" s="132"/>
+      <c r="I23" s="132"/>
+      <c r="J23" s="132"/>
+      <c r="K23" s="132"/>
     </row>
     <row r="24" spans="2:11" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="140" t="s">
+      <c r="C24" s="133" t="s">
         <v>46</v>
       </c>
-      <c r="D24" s="140"/>
-      <c r="E24" s="140"/>
-      <c r="F24" s="140"/>
-      <c r="G24" s="140"/>
-      <c r="H24" s="141"/>
-      <c r="I24" s="141"/>
-      <c r="J24" s="141"/>
-      <c r="K24" s="141"/>
+      <c r="D24" s="133"/>
+      <c r="E24" s="133"/>
+      <c r="F24" s="133"/>
+      <c r="G24" s="133"/>
+      <c r="H24" s="132"/>
+      <c r="I24" s="132"/>
+      <c r="J24" s="132"/>
+      <c r="K24" s="132"/>
     </row>
     <row r="25" spans="2:11" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="144" t="s">
+      <c r="C25" s="129" t="s">
         <v>48</v>
       </c>
-      <c r="D25" s="145"/>
-      <c r="E25" s="145"/>
-      <c r="F25" s="145"/>
-      <c r="G25" s="146"/>
-      <c r="H25" s="141"/>
-      <c r="I25" s="141"/>
-      <c r="J25" s="141"/>
-      <c r="K25" s="141"/>
+      <c r="D25" s="130"/>
+      <c r="E25" s="130"/>
+      <c r="F25" s="130"/>
+      <c r="G25" s="131"/>
+      <c r="H25" s="132"/>
+      <c r="I25" s="132"/>
+      <c r="J25" s="132"/>
+      <c r="K25" s="132"/>
     </row>
     <row r="26" spans="2:11" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C26" s="144" t="s">
+      <c r="C26" s="129" t="s">
         <v>50</v>
       </c>
-      <c r="D26" s="145"/>
-      <c r="E26" s="145"/>
-      <c r="F26" s="145"/>
-      <c r="G26" s="146"/>
-      <c r="H26" s="141"/>
-      <c r="I26" s="141"/>
-      <c r="J26" s="141"/>
-      <c r="K26" s="141"/>
+      <c r="D26" s="130"/>
+      <c r="E26" s="130"/>
+      <c r="F26" s="130"/>
+      <c r="G26" s="131"/>
+      <c r="H26" s="132"/>
+      <c r="I26" s="132"/>
+      <c r="J26" s="132"/>
+      <c r="K26" s="132"/>
     </row>
     <row r="27" spans="2:11" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="144" t="s">
+      <c r="C27" s="129" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="145"/>
-      <c r="E27" s="145"/>
-      <c r="F27" s="145"/>
-      <c r="G27" s="146"/>
-      <c r="H27" s="147"/>
-      <c r="I27" s="148"/>
-      <c r="J27" s="148"/>
-      <c r="K27" s="149"/>
+      <c r="D27" s="130"/>
+      <c r="E27" s="130"/>
+      <c r="F27" s="130"/>
+      <c r="G27" s="131"/>
+      <c r="H27" s="134"/>
+      <c r="I27" s="135"/>
+      <c r="J27" s="135"/>
+      <c r="K27" s="136"/>
     </row>
     <row r="28" spans="2:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C28" s="144" t="s">
+      <c r="C28" s="129" t="s">
         <v>53</v>
       </c>
-      <c r="D28" s="145"/>
-      <c r="E28" s="145"/>
-      <c r="F28" s="145"/>
-      <c r="G28" s="146"/>
-      <c r="H28" s="147"/>
-      <c r="I28" s="148"/>
-      <c r="J28" s="148"/>
-      <c r="K28" s="149"/>
+      <c r="D28" s="130"/>
+      <c r="E28" s="130"/>
+      <c r="F28" s="130"/>
+      <c r="G28" s="131"/>
+      <c r="H28" s="134"/>
+      <c r="I28" s="135"/>
+      <c r="J28" s="135"/>
+      <c r="K28" s="136"/>
     </row>
     <row r="29" spans="2:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="144" t="s">
+      <c r="C29" s="129" t="s">
         <v>54</v>
       </c>
-      <c r="D29" s="145"/>
-      <c r="E29" s="145"/>
-      <c r="F29" s="145"/>
-      <c r="G29" s="146"/>
-      <c r="H29" s="147"/>
-      <c r="I29" s="148"/>
-      <c r="J29" s="148"/>
-      <c r="K29" s="149"/>
+      <c r="D29" s="130"/>
+      <c r="E29" s="130"/>
+      <c r="F29" s="130"/>
+      <c r="G29" s="131"/>
+      <c r="H29" s="134"/>
+      <c r="I29" s="135"/>
+      <c r="J29" s="135"/>
+      <c r="K29" s="136"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="B15:K15"/>
-    <mergeCell ref="B9:K9"/>
-    <mergeCell ref="B10:K10"/>
-    <mergeCell ref="B11:K11"/>
-    <mergeCell ref="B12:K12"/>
-    <mergeCell ref="B13:K13"/>
-    <mergeCell ref="B14:K14"/>
-    <mergeCell ref="B2:K3"/>
-    <mergeCell ref="B6:K6"/>
-    <mergeCell ref="B7:K7"/>
-    <mergeCell ref="B4:J5"/>
-    <mergeCell ref="B8:K8"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="H26:K26"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="H24:K24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="H25:K25"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="H27:K27"/>
-    <mergeCell ref="H28:K28"/>
-    <mergeCell ref="H29:K29"/>
     <mergeCell ref="C23:G23"/>
     <mergeCell ref="H23:K23"/>
     <mergeCell ref="H16:K16"/>
@@ -5285,6 +5261,30 @@
     <mergeCell ref="H22:K22"/>
     <mergeCell ref="C18:G18"/>
     <mergeCell ref="H18:K18"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="H27:K27"/>
+    <mergeCell ref="H28:K28"/>
+    <mergeCell ref="H29:K29"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="H26:K26"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="H24:K24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="H25:K25"/>
+    <mergeCell ref="B2:K3"/>
+    <mergeCell ref="B6:K6"/>
+    <mergeCell ref="B7:K7"/>
+    <mergeCell ref="B4:J5"/>
+    <mergeCell ref="B8:K8"/>
+    <mergeCell ref="B15:K15"/>
+    <mergeCell ref="B9:K9"/>
+    <mergeCell ref="B10:K10"/>
+    <mergeCell ref="B11:K11"/>
+    <mergeCell ref="B12:K12"/>
+    <mergeCell ref="B13:K13"/>
+    <mergeCell ref="B14:K14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="66" orientation="portrait" r:id="rId1"/>

</xml_diff>